<commit_message>
Levantamiento de requerimiento de usuarios inicial de la BANDA, 6 items incluidos
</commit_message>
<xml_diff>
--- a/diseño/historias_plantilla.xlsx
+++ b/diseño/historias_plantilla.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diant\Documents\Trabajo\Curso Desarrollo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prestamour\Documents\desarrollo\PARCIAL\parcialDesarrolloFelipe_Guzman\diseño\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BE123D8D-61D9-4392-87C6-4C06AF9DA141}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1ADA2052-7AFC-4E82-A0AF-1B8DE0A79084}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>id</t>
   </si>
@@ -61,12 +60,57 @@
   </si>
   <si>
     <t>Dificultad</t>
+  </si>
+  <si>
+    <t>OBLIGATORIA</t>
+  </si>
+  <si>
+    <t>BANDA</t>
+  </si>
+  <si>
+    <t>LAS PERSONAS INTERESADAS SEPAN SOBRE NOSOTROS Y NUESTRO RECORRIDO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNA SECCIÓN/PAGINA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNA SECCIÓN/PÁGINA </t>
+  </si>
+  <si>
+    <t>LOS FANS PUEDAN SABER DONDE SERAN LOS PRÓXIMOS CONCIERTOS</t>
+  </si>
+  <si>
+    <t>UNA SECCIÓN/PÁGINA</t>
+  </si>
+  <si>
+    <t>LOS FANS PUEDAN VER EL HISTORIAL DE LOS ÚLTIMOS CONCIERTOS</t>
+  </si>
+  <si>
+    <t>BAJA</t>
+  </si>
+  <si>
+    <t>UNA SECCIÓN/LISTA</t>
+  </si>
+  <si>
+    <t>ENCARGADO DE MERCHANDISING</t>
+  </si>
+  <si>
+    <t>UNA PAGINA</t>
+  </si>
+  <si>
+    <t>SE PUEDA PROMOCIONAR MERCHANDISING DE LA BANDA COMO CAMISAS,DISCOS,ETC.</t>
+  </si>
+  <si>
+    <t>MIS FANS CONOZCAN SOBRE LAS GIRAS QUE HAREMOS</t>
+  </si>
+  <si>
+    <t>LAS PERSONAS INTERESADAS CONOZCAN Y ESCUCHEN ALGUNAS DE NUESTRAS CANCIONES</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -125,12 +169,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -446,57 +493,457 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95F3F769-7A95-40F5-ABEC-F9A1D514FE67}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="3" max="3" width="35" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="26.6640625" customWidth="1"/>
+    <col min="5" max="5" width="82.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="3">
+        <v>90</v>
+      </c>
+      <c r="G3" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="3">
+        <v>100</v>
+      </c>
+      <c r="G4" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="3">
+        <v>100</v>
+      </c>
+      <c r="G5" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="3">
+        <v>20</v>
+      </c>
+      <c r="G6" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="3">
+        <v>90</v>
+      </c>
+      <c r="G7" s="3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="3">
+        <v>80</v>
+      </c>
+      <c r="G8" s="3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
actualizacion excel, creacion de la seccion nosotros,conciertos y musica
</commit_message>
<xml_diff>
--- a/diseño/historias_plantilla.xlsx
+++ b/diseño/historias_plantilla.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prestamour\Documents\desarrollo\PARCIAL\parcialDesarrolloFelipe_Guzman\diseño\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felipe.guzman\Documents\parcialDesarrolloFelipe_Guzman\diseño\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>id</t>
   </si>
@@ -99,9 +99,6 @@
   </si>
   <si>
     <t>SE PUEDA PROMOCIONAR MERCHANDISING DE LA BANDA COMO CAMISAS,DISCOS,ETC.</t>
-  </si>
-  <si>
-    <t>MIS FANS CONOZCAN SOBRE LAS GIRAS QUE HAREMOS</t>
   </si>
   <si>
     <t>LAS PERSONAS INTERESADAS CONOZCAN Y ESCUCHEN ALGUNAS DE NUESTRAS CANCIONES</t>
@@ -110,7 +107,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -174,11 +171,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -497,7 +494,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,10 +506,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -524,16 +521,16 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
@@ -543,407 +540,384 @@
       <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>90</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="2">
+        <v>100</v>
+      </c>
+      <c r="G4" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="2">
+        <v>20</v>
+      </c>
+      <c r="G5" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="3">
-        <v>100</v>
-      </c>
-      <c r="G4" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="3">
-        <v>100</v>
-      </c>
-      <c r="G5" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
+        <v>90</v>
+      </c>
+      <c r="G6" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="3">
-        <v>90</v>
-      </c>
-      <c r="G7" s="3">
+      <c r="D7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="2">
         <v>80</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="3">
+      <c r="G7" s="2">
         <v>80</v>
       </c>
-      <c r="G8" s="3">
-        <v>80</v>
-      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -953,5 +927,6 @@
     <mergeCell ref="G1:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
actualizacion de excel. Creacion de las opciones para redes sociales y mejoras esteticas
</commit_message>
<xml_diff>
--- a/diseño/historias_plantilla.xlsx
+++ b/diseño/historias_plantilla.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>id</t>
   </si>
@@ -90,15 +90,6 @@
   </si>
   <si>
     <t>UNA SECCIÓN/LISTA</t>
-  </si>
-  <si>
-    <t>ENCARGADO DE MERCHANDISING</t>
-  </si>
-  <si>
-    <t>UNA PAGINA</t>
-  </si>
-  <si>
-    <t>SE PUEDA PROMOCIONAR MERCHANDISING DE LA BANDA COMO CAMISAS,DISCOS,ETC.</t>
   </si>
   <si>
     <t>LAS PERSONAS INTERESADAS CONOZCAN Y ESCUCHEN ALGUNAS DE NUESTRAS CANCIONES</t>
@@ -626,7 +617,7 @@
         <v>19</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F6" s="2">
         <v>90</v>
@@ -636,27 +627,13 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="2">
-        <v>80</v>
-      </c>
-      <c r="G7" s="2">
-        <v>80</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>

</xml_diff>